<commit_message>
working normalize excel sheet
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\Cru\missionhub\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379A3E31-39E7-4F42-9600-54A07DB7FCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{A1E9F281-FD67-4A6E-B1FE-94BC63F6F6D2}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="19390" windowHeight="10390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Kevin</t>
   </si>
@@ -109,12 +103,30 @@
   </si>
   <si>
     <t>98982380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brian </t>
+  </si>
+  <si>
+    <t>Lanning</t>
+  </si>
+  <si>
+    <t>8888888888</t>
+  </si>
+  <si>
+    <t>another</t>
+  </si>
+  <si>
+    <t>person</t>
+  </si>
+  <si>
+    <t>988-708-9782</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -505,7 +517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -699,7 +711,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -728,24 +740,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6274FE-8769-48B2-BC11-6CFE84683C44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.3125" customWidth="1"/>
-    <col min="2" max="2" width="14.7890625" customWidth="1"/>
-    <col min="3" max="3" width="10.89453125" customWidth="1"/>
-    <col min="4" max="4" width="11.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.15625" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="43.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="27" t="s">
         <v>13</v>
       </c>
@@ -765,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="24"/>
       <c r="B2" s="24" t="s">
         <v>11</v>
@@ -780,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="24"/>
       <c r="B3" s="24" t="s">
         <v>12</v>
@@ -795,7 +807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="24"/>
       <c r="B4" s="24" t="s">
         <v>5</v>
@@ -808,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="24"/>
       <c r="B5" s="24" t="s">
         <v>16</v>
@@ -820,7 +832,7 @@
       </c>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="24"/>
       <c r="B6" s="24" t="s">
         <v>18</v>
@@ -831,7 +843,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="7"/>
@@ -840,14 +852,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="24"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="24"/>
       <c r="C9" s="7"/>
@@ -856,7 +868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="24"/>
       <c r="B10" s="24" t="s">
         <v>20</v>
@@ -866,7 +878,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="25"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="24"/>
       <c r="B11" s="24" t="s">
         <v>21</v>
@@ -875,7 +887,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="24" t="s">
         <v>22</v>
@@ -885,7 +897,7 @@
       <c r="E12" s="23"/>
       <c r="F12" s="25"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="24" t="s">
         <v>23</v>
@@ -894,22 +906,34 @@
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="24"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="23"/>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="F14" s="25"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="24"/>
       <c r="B15" s="24"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="24"/>
       <c r="C16" s="7"/>
@@ -917,14 +941,14 @@
       <c r="E16" s="23"/>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="24"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="7"/>
@@ -932,195 +956,195 @@
       <c r="E18" s="23"/>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C22" s="5"/>
       <c r="D22" s="8"/>
       <c r="E22" s="20"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C23" s="4"/>
       <c r="D23" s="7"/>
       <c r="E23" s="21"/>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C24" s="5"/>
       <c r="D24" s="8"/>
       <c r="E24" s="20"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C26" s="4"/>
       <c r="D26" s="7"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C27" s="15"/>
       <c r="D27" s="8"/>
       <c r="E27" s="16"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C28" s="4"/>
       <c r="D28" s="7"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C29" s="15"/>
       <c r="D29" s="8"/>
       <c r="E29" s="16"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C30" s="4"/>
       <c r="D30" s="7"/>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C31" s="15"/>
       <c r="D31" s="8"/>
       <c r="E31" s="16"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C32" s="4"/>
       <c r="D32" s="7"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="15"/>
       <c r="D33" s="8"/>
       <c r="E33" s="16"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C34" s="4"/>
       <c r="D34" s="7"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="23"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="23"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="23"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="23"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="23"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
       <c r="D42" s="9"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C43" s="1"/>
       <c r="D43" s="9"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D62" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearranged excel sheet and added gender
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Kevin</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Kevin Horn</t>
   </si>
   <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
     <t>Phone Number</t>
   </si>
   <si>
@@ -121,6 +118,30 @@
   </si>
   <si>
     <t>988-708-9782</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Gender formatted</t>
   </si>
 </sst>
 </file>
@@ -156,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -324,11 +345,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -341,9 +380,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,32 +399,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -399,11 +422,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,435 +758,417 @@
 </a:theme>
 </file>
 
-<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
-<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="875" row="5">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </wetp:taskpane>
-</wetp:taskpanes>
-</file>
-
-<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{E6EA0BE0-DDBA-4B8B-BF40-2CD2D4DBC857}">
-  <we:reference id="wa104381701" version="1.0.0.2" store="en-US" storeType="OMEX"/>
-  <we:alternateReferences>
-    <we:reference id="wa104381701" version="1.0.0.2" store="WA104381701" storeType="OMEX"/>
-  </we:alternateReferences>
-  <we:properties/>
-  <we:bindings>
-    <we:binding id="currentSelection" type="table" appref="{2105D1D0-6DFA-4A12-BB12-F853D08C7FC0}"/>
-  </we:bindings>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</we:webextension>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12" style="18" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="29" t="s">
+      <c r="C5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="25"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
       <c r="B6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="18"/>
+      <c r="B7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="18"/>
+      <c r="B8" s="24"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="18"/>
+      <c r="B9" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="23" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="18"/>
+      <c r="B14" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="23" t="s">
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="18"/>
+      <c r="B15" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="24"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="18"/>
       <c r="B16" s="24"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="24"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="24"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="23"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="24"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="24"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="25"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="24"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="24"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="23"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="24"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="24"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="23"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="23"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="5"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="22"/>
+      <c r="B22" s="16"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="10"/>
+      <c r="B23" s="17"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C24" s="5"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="11"/>
+      <c r="B24" s="16"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
+      <c r="B25" s="26"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C26" s="4"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="17"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C27" s="15"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C28" s="4"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="17"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C29" s="15"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C30" s="4"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="17"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C31" s="15"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="4"/>
-      <c r="D32" s="7"/>
+      <c r="B32" s="17"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C33" s="15"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C34" s="4"/>
-      <c r="D34" s="7"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="17"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="23"/>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="23"/>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="23"/>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="23"/>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="23"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C42" s="1"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C43" s="1"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D46" s="10"/>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D50" s="10"/>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D52" s="10"/>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D55" s="10"/>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D56" s="10"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D62" s="11"/>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="27"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="27"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="24"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="24"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="24"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="24"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="24"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="2"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="2"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E50" s="9"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E56" s="9"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E60" s="9"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E61" s="9"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E62" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding contacts with labels works
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Kevin</t>
   </si>
@@ -752,7 +752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,7 +763,7 @@
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,6 +942,9 @@
       <c r="B14" s="24" t="s">
         <v>27</v>
       </c>
+      <c r="C14" s="18" t="s">
+        <v>36</v>
+      </c>
       <c r="D14" s="6" t="s">
         <v>25</v>
       </c>

</xml_diff>